<commit_message>
Updated the applied model configurations
</commit_message>
<xml_diff>
--- a/chapters/applied/docs/model-configuration.xlsx
+++ b/chapters/applied/docs/model-configuration.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/PhD/Thesis/chapters/applied/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Thesis/chapters/applied/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="3720" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="2520" yWindow="2460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="basic-biology" sheetId="1" r:id="rId1"/>
+    <sheet name="spawning" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -76,11 +77,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Demersal eggs</t>
+Pelagic eggs</t>
         </r>
       </text>
     </comment>
-    <comment ref="A30" authorId="0">
+    <comment ref="A18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -109,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>parameters</t>
   </si>
@@ -156,15 +157,9 @@
     <t>olfactory-sense</t>
   </si>
   <si>
-    <t>5km</t>
-  </si>
-  <si>
     <t>settlement-sense</t>
   </si>
   <si>
-    <t>2km</t>
-  </si>
-  <si>
     <t>ovm matrix</t>
   </si>
   <si>
@@ -183,18 +178,6 @@
     <t>deep</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>diel matrix</t>
-  </si>
-  <si>
-    <t>night</t>
-  </si>
-  <si>
-    <t>day</t>
-  </si>
-  <si>
     <t>Epinephelus daemelii</t>
   </si>
   <si>
@@ -204,15 +187,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>depth</t>
-  </si>
-  <si>
     <t>number</t>
   </si>
   <si>
@@ -228,10 +202,100 @@
     <t>end</t>
   </si>
   <si>
-    <t>northern nsw</t>
-  </si>
-  <si>
-    <t>orientation</t>
+    <t>marine park</t>
+  </si>
+  <si>
+    <t>critical swimming speed</t>
+  </si>
+  <si>
+    <t>in situ potential</t>
+  </si>
+  <si>
+    <t>endurance</t>
+  </si>
+  <si>
+    <t>Leis 2009</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>cape byron</t>
+  </si>
+  <si>
+    <t>nsw-mpa</t>
+  </si>
+  <si>
+    <t>solitary islands</t>
+  </si>
+  <si>
+    <t>port stephens</t>
+  </si>
+  <si>
+    <t>lord howe</t>
+  </si>
+  <si>
+    <t>jervis bay</t>
+  </si>
+  <si>
+    <t>middleton reef</t>
+  </si>
+  <si>
+    <t>elizabeth reef</t>
+  </si>
+  <si>
+    <t>commonwealth</t>
+  </si>
+  <si>
+    <t>pinnacle reefs</t>
+  </si>
+  <si>
+    <t>cod grounds</t>
+  </si>
+  <si>
+    <t>specific sites</t>
+  </si>
+  <si>
+    <t>north solitary island, south solitary island, north west rock, pimpernal rock, fish rock</t>
+  </si>
+  <si>
+    <t>locations</t>
+  </si>
+  <si>
+    <t>hunter</t>
+  </si>
+  <si>
+    <t>hawkesbury shelf</t>
+  </si>
+  <si>
+    <t>nsw-aquatic</t>
+  </si>
+  <si>
+    <t>norfolk island</t>
+  </si>
+  <si>
+    <t>Cuhna 2013</t>
+  </si>
+  <si>
+    <t>Cuhna 2014</t>
+  </si>
+  <si>
+    <t>Cuhna 2015</t>
+  </si>
+  <si>
+    <t>Francis 2016</t>
+  </si>
+  <si>
+    <t>Francis 2017</t>
+  </si>
+  <si>
+    <t>Leis 2010</t>
+  </si>
+  <si>
+    <t>Leis 2011</t>
+  </si>
+  <si>
+    <t>April-May is annecdotal from Harasti</t>
   </si>
 </sst>
 </file>
@@ -283,7 +347,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,6 +366,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -315,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -336,6 +406,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,7 +704,7 @@
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,31 +715,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -673,39 +753,48 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -713,352 +802,451 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2">
-        <v>62</v>
-      </c>
-      <c r="H17" s="7">
-        <v>38078</v>
-      </c>
-      <c r="I17" s="7">
-        <v>38138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2">
-        <v>62</v>
-      </c>
-      <c r="H18" s="7">
-        <v>38443</v>
-      </c>
-      <c r="I18" s="7">
-        <v>38503</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F19" s="2">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2">
-        <v>62</v>
-      </c>
-      <c r="H19" s="7">
-        <v>38808</v>
-      </c>
-      <c r="I19" s="7">
-        <v>38868</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2">
-        <v>62</v>
-      </c>
-      <c r="H20" s="7">
-        <v>39173</v>
-      </c>
-      <c r="I20" s="7">
-        <v>39233</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2">
-        <v>62</v>
-      </c>
-      <c r="H21" s="7">
-        <v>39539</v>
-      </c>
-      <c r="I21" s="7">
-        <v>39599</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22" s="2">
-        <v>62</v>
-      </c>
-      <c r="H22" s="7">
-        <v>39904</v>
-      </c>
-      <c r="I22" s="7">
-        <v>39964</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1</v>
-      </c>
-      <c r="G23" s="2">
-        <v>62</v>
-      </c>
-      <c r="H23" s="7">
-        <v>40269</v>
-      </c>
-      <c r="I23" s="7">
-        <v>40329</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F24" s="2">
-        <v>1</v>
-      </c>
-      <c r="G24" s="2">
-        <v>62</v>
-      </c>
-      <c r="H24" s="7">
-        <v>40634</v>
-      </c>
-      <c r="I24" s="7">
-        <v>40694</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1</v>
-      </c>
-      <c r="G25" s="2">
-        <v>62</v>
-      </c>
-      <c r="H25" s="7">
-        <v>41000</v>
-      </c>
-      <c r="I25" s="7">
-        <v>41060</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="C18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="D18" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="B19" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="B20" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="D31" s="2">
+      <c r="B21" s="2">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0.35</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C33" s="2">
+      <c r="C21" s="2">
         <v>0.375</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D21" s="2">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="2">
-        <f>SUM(B31:B33)</f>
-        <v>1</v>
-      </c>
-      <c r="C34" s="2">
-        <f t="shared" ref="C34:D34" si="0">SUM(C31:C33)</f>
-        <v>1</v>
-      </c>
-      <c r="D34" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="C36" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C37" s="2">
-        <v>0.9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>62</v>
+      </c>
+      <c r="E3" s="7">
+        <v>38078</v>
+      </c>
+      <c r="F3" s="7">
+        <v>38138</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>62</v>
+      </c>
+      <c r="E4" s="7">
+        <v>38443</v>
+      </c>
+      <c r="F4" s="7">
+        <v>38503</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>62</v>
+      </c>
+      <c r="E5" s="7">
+        <v>38808</v>
+      </c>
+      <c r="F5" s="7">
+        <v>38868</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>62</v>
+      </c>
+      <c r="E6" s="7">
+        <v>39173</v>
+      </c>
+      <c r="F6" s="7">
+        <v>39233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>62</v>
+      </c>
+      <c r="E7" s="7">
+        <v>39539</v>
+      </c>
+      <c r="F7" s="7">
+        <v>39599</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>62</v>
+      </c>
+      <c r="E8" s="7">
+        <v>39904</v>
+      </c>
+      <c r="F8" s="7">
+        <v>39964</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>62</v>
+      </c>
+      <c r="E9" s="7">
+        <v>40269</v>
+      </c>
+      <c r="F9" s="7">
+        <v>40329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>62</v>
+      </c>
+      <c r="E10" s="7">
+        <v>40634</v>
+      </c>
+      <c r="F10" s="7">
+        <v>40694</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>62</v>
+      </c>
+      <c r="E11" s="7">
+        <v>41000</v>
+      </c>
+      <c r="F11" s="7">
+        <v>41060</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Scripts and configs for applied chapter
</commit_message>
<xml_diff>
--- a/chapters/applied/docs/model-configuration.xlsx
+++ b/chapters/applied/docs/model-configuration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="2460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="basic-biology" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
   <si>
     <t>parameters</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>mortality</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>preflexion-mean</t>
@@ -689,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,7 +717,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -731,7 +728,7 @@
         <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -742,53 +739,53 @@
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
+      <c r="B5" s="2">
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -796,78 +793,78 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="2">
         <v>0.3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2">
         <v>0.16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2">
         <v>0.5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2">
         <v>0.45</v>
@@ -881,7 +878,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2">
         <v>0.45</v>
@@ -895,7 +892,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2">
         <v>0.1</v>
@@ -917,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -930,32 +927,32 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2">
         <v>10000</v>
@@ -973,12 +970,12 @@
         <v>38138</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2">
         <v>10000</v>
@@ -998,7 +995,7 @@
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2">
         <v>10000</v>
@@ -1018,7 +1015,7 @@
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2">
         <v>10000</v>
@@ -1038,7 +1035,7 @@
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2">
         <v>10000</v>
@@ -1058,7 +1055,7 @@
     </row>
     <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2">
         <v>10000</v>
@@ -1078,7 +1075,7 @@
     </row>
     <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2">
         <v>10000</v>
@@ -1098,7 +1095,7 @@
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2">
         <v>10000</v>
@@ -1118,7 +1115,7 @@
     </row>
     <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2">
         <v>10000</v>
@@ -1138,112 +1135,112 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
         <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
-      </c>
-      <c r="B22" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
         <v>51</v>
-      </c>
-      <c r="B25" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on the applied chapter analysis
</commit_message>
<xml_diff>
--- a/chapters/applied/docs/model-configuration.xlsx
+++ b/chapters/applied/docs/model-configuration.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Thesis/chapters/applied/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/PhD/Thesis/chapters/applied/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="4480" yWindow="1860" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="basic-biology" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t>parameters</t>
   </si>
@@ -293,6 +293,36 @@
   </si>
   <si>
     <t>April-May is annecdotal from Harasti</t>
+  </si>
+  <si>
+    <t>site_code</t>
+  </si>
+  <si>
+    <t>NSW02</t>
+  </si>
+  <si>
+    <t>NSW05</t>
+  </si>
+  <si>
+    <t>NSW09</t>
+  </si>
+  <si>
+    <t>NSW18</t>
+  </si>
+  <si>
+    <t>NSW13</t>
+  </si>
+  <si>
+    <t>NSW19</t>
+  </si>
+  <si>
+    <t>NSW07</t>
+  </si>
+  <si>
+    <t>NSW10</t>
+  </si>
+  <si>
+    <t>NSW11</t>
   </si>
 </sst>
 </file>
@@ -686,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -914,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1148,6 +1178,9 @@
       <c r="C15" s="9" t="s">
         <v>46</v>
       </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -1156,8 +1189,11 @@
       <c r="B16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
@@ -1167,8 +1203,11 @@
       <c r="C17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -1178,64 +1217,88 @@
       <c r="C18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B25" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>

</xml_diff>